<commit_message>
TCER in pdf format added
</commit_message>
<xml_diff>
--- a/Catalog-Service/src/main/resources/TCER/Catalog-TCER.xlsx
+++ b/Catalog-Service/src/main/resources/TCER/Catalog-TCER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suyesh\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E35EF9F9-483E-4C6D-98A0-C843138EF05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F5C13F-941C-450F-8B2A-638E07EE8198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB40684C-EEE6-4A15-AD77-E52110D281A1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>S. No.</t>
   </si>
@@ -65,40 +65,70 @@
     <t>T002</t>
   </si>
   <si>
-    <t>listAllProducts()</t>
-  </si>
-  <si>
     <t>PRODUCT_BY_CODE</t>
   </si>
   <si>
     <t>Catalog-Service</t>
   </si>
   <si>
-    <t>getProductByCode("P001")</t>
-  </si>
-  <si>
-    <t>getProductByCode("P111")</t>
-  </si>
-  <si>
-    <t>findAll()</t>
-  </si>
-  <si>
-    <t>findById("P001")</t>
-  </si>
-  <si>
-    <t>findById("P111")</t>
-  </si>
-  <si>
     <t>List&lt;Product&gt;</t>
   </si>
   <si>
-    <t>empty List</t>
-  </si>
-  <si>
     <t>some product</t>
   </si>
   <si>
     <t>no product</t>
+  </si>
+  <si>
+    <t>T003</t>
+  </si>
+  <si>
+    <t>T004</t>
+  </si>
+  <si>
+    <t>product1</t>
+  </si>
+  <si>
+    <t>product2</t>
+  </si>
+  <si>
+    <t>product3</t>
+  </si>
+  <si>
+    <t>T005</t>
+  </si>
+  <si>
+    <t>catalogDao.findAll()</t>
+  </si>
+  <si>
+    <t>catalogDao.findByCode("P001")</t>
+  </si>
+  <si>
+    <t>catalogDao.findByCode("P002")</t>
+  </si>
+  <si>
+    <t>catalogDao.findByCode("P003")</t>
+  </si>
+  <si>
+    <t>catalogDao.findByCode("P111")</t>
+  </si>
+  <si>
+    <t>catalogDao.findByCode("P112")</t>
+  </si>
+  <si>
+    <t>catalogService.listAllProducts()</t>
+  </si>
+  <si>
+    <t>catalogService.getProductByCode("P002")</t>
+  </si>
+  <si>
+    <t>catalogService.getProductByCode("P001")</t>
+  </si>
+  <si>
+    <t>catalogService.getProductByCode("P111")</t>
+  </si>
+  <si>
+    <t>catalogService.getProductByCode("P112")</t>
   </si>
 </sst>
 </file>
@@ -453,17 +483,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A44A080-376B-4663-A3BC-9FF40AEC89D0}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25.44140625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="39.88671875" customWidth="1"/>
     <col min="5" max="5" width="30.77734375" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
@@ -504,10 +534,10 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -515,16 +545,16 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -532,16 +562,16 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -549,109 +579,160 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>0</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>3</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E15" t="s">
         <v>4</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F15" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
+      <c r="D17" t="s">
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>4</v>
       </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
         <v>14</v>
       </c>
-      <c r="E18" t="s">
-        <v>21</v>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>